<commit_message>
Added models in inventory service
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Spring-Boot\spring-ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F5AC2B-AB70-4243-AA19-C6FC148CC012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6772DF3-D035-4B56-ACCA-53BA5A0AC695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -287,9 +287,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,6 +295,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,13 +617,13 @@
       </c>
     </row>
     <row r="2" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="11">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -638,9 +638,9 @@
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
       <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
@@ -653,13 +653,13 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="5">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="11">
+        <v>2</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -674,9 +674,9 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
       <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
@@ -689,11 +689,11 @@
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="5">
+      <c r="C6" s="11">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
       <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
@@ -704,9 +704,9 @@
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
       <c r="F7" s="2" t="s">
         <v>3</v>
       </c>
@@ -717,11 +717,11 @@
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="5">
+      <c r="C8" s="11">
         <v>4</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
       <c r="F8" s="2" t="s">
         <v>2</v>
       </c>
@@ -732,9 +732,9 @@
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
       <c r="F9" s="2" t="s">
         <v>3</v>
       </c>
@@ -745,11 +745,11 @@
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="5">
+      <c r="C10" s="11">
         <v>5</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
       <c r="F10" s="2" t="s">
         <v>2</v>
       </c>
@@ -760,9 +760,9 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
       <c r="F11" s="2" t="s">
         <v>3</v>
       </c>
@@ -773,11 +773,11 @@
       </c>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="5">
+      <c r="C12" s="11">
         <v>6</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
       <c r="F12" s="2" t="s">
         <v>2</v>
       </c>
@@ -788,9 +788,9 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
       <c r="F13" s="2" t="s">
         <v>3</v>
       </c>
@@ -801,11 +801,11 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="5">
+      <c r="C14" s="11">
         <v>7</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="2" t="s">
         <v>2</v>
       </c>
@@ -816,9 +816,9 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
       <c r="F15" s="2" t="s">
         <v>3</v>
       </c>
@@ -829,11 +829,11 @@
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="5">
+      <c r="C16" s="11">
         <v>8</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
       <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
@@ -844,9 +844,9 @@
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
       <c r="F17" s="2" t="s">
         <v>3</v>
       </c>
@@ -858,30 +858,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -895,7 +895,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,7 +921,7 @@
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -949,7 +949,7 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="4">
@@ -979,7 +979,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="4">
@@ -1007,7 +1007,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C5" s="4">
@@ -1035,7 +1035,7 @@
       <c r="A6">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="4">
@@ -1071,7 +1071,7 @@
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C7" s="4">
@@ -1099,7 +1099,7 @@
       <c r="A8">
         <v>1</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C8" s="4">
@@ -1127,7 +1127,7 @@
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="4">
@@ -1155,7 +1155,7 @@
       <c r="A10">
         <v>1</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="4">
@@ -1183,7 +1183,7 @@
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="4">
@@ -1213,7 +1213,7 @@
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="4">
@@ -1243,7 +1243,7 @@
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="4">
@@ -1273,7 +1273,7 @@
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="C14" s="4">
@@ -1303,7 +1303,7 @@
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="4">
@@ -1335,7 +1335,7 @@
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="4">
@@ -1369,7 +1369,7 @@
       <c r="A17">
         <v>2</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C17" s="4">
@@ -1399,7 +1399,7 @@
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="4">
@@ -1427,7 +1427,7 @@
       <c r="A19">
         <v>2</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C19" s="4">
@@ -1455,7 +1455,7 @@
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="4">
@@ -1480,7 +1480,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C21" s="4">

</xml_diff>